<commit_message>
fix a few logic in answer and vuln sql injection and xss
</commit_message>
<xml_diff>
--- a/public/import_quiz.xlsx
+++ b/public/import_quiz.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>question</t>
   </si>
@@ -27,12 +27,6 @@
     <t>answer</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>optionA</t>
   </si>
   <si>
@@ -45,41 +39,52 @@
     <t>optionD</t>
   </si>
   <si>
-    <t>Theo em việc tạo thư mục có tác dụng như thế nào?</t>
-  </si>
-  <si>
-    <t>Tạo thư mục giúp em lưu trữ thông tin và tìm kiếm thông tin một cách dễ dàng.</t>
-  </si>
-  <si>
-    <t>Tạo thư mục không lưu trữ được thông tin.</t>
-  </si>
-  <si>
-    <t>Tạo thư mục chỉ lưu trữ được các bài hát.</t>
-  </si>
-  <si>
-    <t>Cả A,B,C đều đúng</t>
-  </si>
-  <si>
-    <t>Thư mục là một phân vùng hình thức trên đĩa để việc lưu trữ các tập tin có hệ thống. Người sử dụng có thể phân một đĩa ra thành nhiều vùng riêng biệt, trong mỗi vùng có thể là lưu trữ một phần mềm nào đó hoặc các tập tin riêng của từng người sử dụng ... Mỗi vùng gọi là một thư mục.</t>
-  </si>
-  <si>
-    <t>Chuột, bàn phím thuộc nhóm thiết bị gì?</t>
-  </si>
-  <si>
-    <t>Nhóm thiết bị ra</t>
-  </si>
-  <si>
-    <t>Nhóm thiết bị vào.</t>
-  </si>
-  <si>
-    <t>Nhóm thiết bị truyền thông</t>
-  </si>
-  <si>
-    <t>Nhóm thiết bị vào/ra</t>
-  </si>
-  <si>
-    <t>Một số thiết bị đầu vào máy tính quan trọng được liệt kê dưới đây:
-Chuột, Bàn phím, Máy quét, Micro, Webcam</t>
+    <t>hide_option</t>
+  </si>
+  <si>
+    <t>Lưu ý: Trường hide_option nếu bằng 1 thì sẽ ẩn các tùy chọn, nếu bằng 0 thì không ẩn. Và bỏ qua dòng 1 này. Mặc định là không ẩn, nếu không ẩn thì bỏ trường đó đi.</t>
+  </si>
+  <si>
+    <t>Tại sao đến năm 1965, Mĩ phải chuyển sang thực hiện chiến lược “Chiến tranh cục bộ”?</t>
+  </si>
+  <si>
+    <t>Mĩ muốn nhanh chóng kết thúc chiến tranh Việt Nam.</t>
+  </si>
+  <si>
+    <t>Mĩ muốn mở rộng và quốc tế hóa chiến tranh Việt Nam</t>
+  </si>
+  <si>
+    <t>Mĩ lo ngại ủng hộ của Trung Quốc và Liên Xô cho cuộc kháng chiến của nhân dân ta</t>
+  </si>
+  <si>
+    <t>Chiến lược “Chiến tranh đặc biệt” đã bị phá sản hoàn toàn.</t>
+  </si>
+  <si>
+    <t>Việt Nam gia nhập ASEAN có ý nghĩa là</t>
+  </si>
+  <si>
+    <t>ASEAN đã trở thành một liên minh kinh tế - chính trị</t>
+  </si>
+  <si>
+    <t>Chứng tỏ sự đối đầu về ý thực hệ tư tưởng – chính trị - quân sự</t>
+  </si>
+  <si>
+    <t>mở ra triển vọng cho sự liên kết toàn khu vực Đông Nam Á.</t>
+  </si>
+  <si>
+    <t>Chứng tỏ sự hợp tác giữa các thành viên ASEAN ngày càng có hiệu quả.</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Đến năm 1965, Mĩ phải chuyển sang thực hiện chiến lược “Chiến tranh cục bộ” vì  chiến lược “Chiến tranh đặc biệt” đã bị phá sản hoàn toàn.</t>
+  </si>
+  <si>
+    <t>Việt Nam gia nhập ASEAN có ý nghĩa là mở ra triển vọng cho sự liên kết toàn khu vực Đông Nam Á.</t>
   </si>
 </sst>
 </file>
@@ -115,10 +120,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,94 +429,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="40.125" customWidth="1"/>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="2" max="2" width="27.875" customWidth="1"/>
     <col min="3" max="3" width="24.125" customWidth="1"/>
     <col min="4" max="4" width="20.375" customWidth="1"/>
     <col min="5" max="5" width="19.625" customWidth="1"/>
     <col min="6" max="6" width="16.125" customWidth="1"/>
     <col min="7" max="7" width="28.375" customWidth="1"/>
+    <col min="8" max="8" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F4" t="s">
         <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:L1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 

</xml_diff>